<commit_message>
ft_printf testing in progress
</commit_message>
<xml_diff>
--- a/ft_printf/ft_printf specs and dvlpt tracking.xlsx
+++ b/ft_printf/ft_printf specs and dvlpt tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkara\42\ft_printf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06CDAAD-A983-4FE1-9837-84F9AE3AB63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D1E0DB-8C71-4815-8D88-B6B92836EAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="modifs libft" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Conversion specifier</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>modification type</t>
+  </si>
+  <si>
+    <t>return int et write (null) si s == NULL</t>
+  </si>
+  <si>
+    <t>ft_put_uint_fd</t>
   </si>
 </sst>
 </file>
@@ -163,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -186,11 +192,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -198,6 +215,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +533,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B13" sqref="B13:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +626,10 @@
       <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3">
+        <f>-2147483648 + 4294967295+1</f>
+        <v>2147483648</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -656,16 +677,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -689,7 +710,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -705,6 +726,14 @@
         <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>